<commit_message>
Update the submission sheet
Signed-off-by: Amar Tumballi <amar@kadalu.io>
</commit_message>
<xml_diff>
--- a/dhiway/Submission_Sheet.xlsx
+++ b/dhiway/Submission_Sheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
   <si>
     <r>
       <rPr>
@@ -105,19 +105,19 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>https://github.com/dhiway/innovation-hackathon-jan22 - Assumption section</t>
+    <t>https://github.com/dhiway/innovation-hackathon-jan22/blob/main/dhiway/Dhiway-Challenge09.md#assumptions</t>
   </si>
   <si>
-    <t>https://github.com/dhiway/innovation-hackathon-jan22</t>
+    <t>https://github.com/dhiway/innovation-hackathon-jan22/blob/main/dhiway/Dhiway-Challenge09.md#demo-flow</t>
+  </si>
+  <si>
+    <t>https://github.com/dhiway/innovation-hackathon-jan22/blob/main/dhiway/Dhiway-Challenge09.md#demo-setup</t>
   </si>
   <si>
     <t>Available</t>
   </si>
   <si>
-    <t>Yes - Need to Architect properly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proof of Stake, </t>
+    <t>https://github.com/dhiway/innovation-hackathon-jan22/blob/main/dhiway/Dhiway-Challenge09.md#network-operations</t>
   </si>
   <si>
     <t>b</t>
@@ -138,6 +138,21 @@
     <t>Create e-commerce solutions for the decentralized web</t>
   </si>
   <si>
+    <t>https://github.com/dhiway/innovation-hackathon-jan22/blob/main/dhiway/Dhiway-Challenge10.md#assumptions</t>
+  </si>
+  <si>
+    <t>https://apps.cord.network/#/explorer</t>
+  </si>
+  <si>
+    <t>https://github.com/dhiway/cord/tree/ondc-hackathon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes </t>
+  </si>
+  <si>
+    <t>https://github.com/dhiway/innovation-hackathon-jan22/blob/main/dhiway/CORD_Lightpaper_v1.pdf</t>
+  </si>
+  <si>
     <t>Beckn Protocol Evolution</t>
   </si>
   <si>
@@ -154,7 +169,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -205,7 +220,14 @@
     </font>
     <font>
       <u/>
+      <sz val="9.0"/>
       <color rgb="FF1155CC"/>
+      <name val="Lato"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9.0"/>
+      <color rgb="FF0000FF"/>
       <name val="Lato"/>
     </font>
     <font>
@@ -516,12 +538,12 @@
     <xf borderId="4" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="4" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1146,21 +1168,21 @@
         <v>26</v>
       </c>
       <c r="I9" s="36" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J9" s="37" t="s">
         <v>24</v>
       </c>
       <c r="K9" s="37" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L9" s="37" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="M9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="N9" s="37" t="s">
+      <c r="N9" s="38" t="s">
         <v>29</v>
       </c>
       <c r="O9" s="22"/>
@@ -1184,9 +1206,9 @@
       <c r="AG9" s="22"/>
     </row>
     <row r="10">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
       <c r="D10" s="31" t="s">
         <v>30</v>
       </c>
@@ -1196,14 +1218,14 @@
       <c r="F10" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
       <c r="O10" s="22"/>
       <c r="P10" s="22"/>
       <c r="Q10" s="22"/>
@@ -1225,9 +1247,9 @@
       <c r="AG10" s="22"/>
     </row>
     <row r="11">
-      <c r="A11" s="38"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
       <c r="D11" s="31" t="s">
         <v>31</v>
       </c>
@@ -1237,14 +1259,14 @@
       <c r="F11" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
       <c r="O11" s="22"/>
       <c r="P11" s="22"/>
       <c r="Q11" s="22"/>
@@ -1266,24 +1288,26 @@
       <c r="AG11" s="22"/>
     </row>
     <row r="12">
-      <c r="A12" s="39"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
       <c r="D12" s="31" t="s">
         <v>32</v>
       </c>
       <c r="E12" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="40"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
+      <c r="F12" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="40"/>
       <c r="O12" s="22"/>
       <c r="P12" s="22"/>
       <c r="Q12" s="22"/>
@@ -1355,15 +1379,33 @@
       <c r="E14" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="40"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="42"/>
-      <c r="N14" s="42"/>
+      <c r="F14" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="L14" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="M14" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="N14" s="36" t="s">
+        <v>40</v>
+      </c>
       <c r="O14" s="22"/>
       <c r="P14" s="22"/>
       <c r="Q14" s="22"/>
@@ -1385,24 +1427,26 @@
       <c r="AG14" s="22"/>
     </row>
     <row r="15">
-      <c r="A15" s="38"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
       <c r="D15" s="31" t="s">
         <v>30</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="40"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="38"/>
+      <c r="F15" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="39"/>
+      <c r="N15" s="39"/>
       <c r="O15" s="22"/>
       <c r="P15" s="22"/>
       <c r="Q15" s="22"/>
@@ -1424,24 +1468,26 @@
       <c r="AG15" s="22"/>
     </row>
     <row r="16">
-      <c r="A16" s="38"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
+      <c r="A16" s="39"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
       <c r="D16" s="31" t="s">
         <v>31</v>
       </c>
       <c r="E16" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="40"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="38"/>
-      <c r="M16" s="38"/>
-      <c r="N16" s="38"/>
+      <c r="F16" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
       <c r="O16" s="22"/>
       <c r="P16" s="22"/>
       <c r="Q16" s="22"/>
@@ -1463,24 +1509,26 @@
       <c r="AG16" s="22"/>
     </row>
     <row r="17">
-      <c r="A17" s="39"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
       <c r="D17" s="31" t="s">
         <v>32</v>
       </c>
       <c r="E17" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="40"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="39"/>
+      <c r="F17" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="40"/>
       <c r="O17" s="22"/>
       <c r="P17" s="22"/>
       <c r="Q17" s="22"/>
@@ -1541,10 +1589,10 @@
         <v>11.0</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D19" s="31" t="s">
         <v>22</v>
@@ -1582,9 +1630,9 @@
       <c r="AG19" s="22"/>
     </row>
     <row r="20">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
       <c r="D20" s="31" t="s">
         <v>30</v>
       </c>
@@ -1592,14 +1640,14 @@
         <v>23</v>
       </c>
       <c r="F20" s="35"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="38"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="39"/>
       <c r="O20" s="22"/>
       <c r="P20" s="22"/>
       <c r="Q20" s="22"/>
@@ -1621,9 +1669,9 @@
       <c r="AG20" s="22"/>
     </row>
     <row r="21">
-      <c r="A21" s="38"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
+      <c r="A21" s="39"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
       <c r="D21" s="31" t="s">
         <v>31</v>
       </c>
@@ -1631,14 +1679,14 @@
         <v>23</v>
       </c>
       <c r="F21" s="35"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="38"/>
-      <c r="L21" s="38"/>
-      <c r="M21" s="38"/>
-      <c r="N21" s="38"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
       <c r="O21" s="22"/>
       <c r="P21" s="22"/>
       <c r="Q21" s="22"/>
@@ -1660,9 +1708,9 @@
       <c r="AG21" s="22"/>
     </row>
     <row r="22">
-      <c r="A22" s="38"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="38"/>
+      <c r="A22" s="39"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
       <c r="D22" s="31" t="s">
         <v>32</v>
       </c>
@@ -1670,14 +1718,14 @@
         <v>23</v>
       </c>
       <c r="F22" s="35"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="38"/>
-      <c r="M22" s="38"/>
-      <c r="N22" s="38"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="39"/>
       <c r="O22" s="22"/>
       <c r="P22" s="22"/>
       <c r="Q22" s="22"/>
@@ -1699,24 +1747,24 @@
       <c r="AG22" s="22"/>
     </row>
     <row r="23">
-      <c r="A23" s="38"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
+      <c r="A23" s="39"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
       <c r="D23" s="31" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E23" s="31" t="s">
         <v>23</v>
       </c>
       <c r="F23" s="35"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="38"/>
-      <c r="K23" s="38"/>
-      <c r="L23" s="38"/>
-      <c r="M23" s="38"/>
-      <c r="N23" s="38"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="39"/>
       <c r="O23" s="22"/>
       <c r="P23" s="22"/>
       <c r="Q23" s="22"/>
@@ -1738,24 +1786,24 @@
       <c r="AG23" s="22"/>
     </row>
     <row r="24">
-      <c r="A24" s="39"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
       <c r="D24" s="31" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E24" s="31" t="s">
         <v>23</v>
       </c>
       <c r="F24" s="35"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="39"/>
-      <c r="N24" s="39"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="40"/>
       <c r="O24" s="22"/>
       <c r="P24" s="22"/>
       <c r="Q24" s="22"/>
@@ -35758,7 +35806,12 @@
     <hyperlink r:id="rId2" ref="G9"/>
     <hyperlink r:id="rId3" ref="H9"/>
     <hyperlink r:id="rId4" ref="I9"/>
+    <hyperlink r:id="rId5" location="network-operations" ref="N9"/>
+    <hyperlink r:id="rId6" location="assumptions" ref="G14"/>
+    <hyperlink r:id="rId7" location="/explorer" ref="H14"/>
+    <hyperlink r:id="rId8" ref="I14"/>
+    <hyperlink r:id="rId9" ref="N14"/>
   </hyperlinks>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update the submission sheet (#5)
</commit_message>
<xml_diff>
--- a/dhiway/Submission_Sheet.xlsx
+++ b/dhiway/Submission_Sheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
   <si>
     <r>
       <rPr>
@@ -105,19 +105,19 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>https://github.com/dhiway/innovation-hackathon-jan22 - Assumption section</t>
+    <t>https://github.com/dhiway/innovation-hackathon-jan22/blob/main/dhiway/Dhiway-Challenge09.md#assumptions</t>
   </si>
   <si>
-    <t>https://github.com/dhiway/innovation-hackathon-jan22</t>
+    <t>https://github.com/dhiway/innovation-hackathon-jan22/blob/main/dhiway/Dhiway-Challenge09.md#demo-flow</t>
+  </si>
+  <si>
+    <t>https://github.com/dhiway/innovation-hackathon-jan22/blob/main/dhiway/Dhiway-Challenge09.md#demo-setup</t>
   </si>
   <si>
     <t>Available</t>
   </si>
   <si>
-    <t>Yes - Need to Architect properly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proof of Stake, </t>
+    <t>https://github.com/dhiway/innovation-hackathon-jan22/blob/main/dhiway/Dhiway-Challenge09.md#network-operations</t>
   </si>
   <si>
     <t>b</t>
@@ -138,6 +138,21 @@
     <t>Create e-commerce solutions for the decentralized web</t>
   </si>
   <si>
+    <t>https://github.com/dhiway/innovation-hackathon-jan22/blob/main/dhiway/Dhiway-Challenge10.md#assumptions</t>
+  </si>
+  <si>
+    <t>https://apps.cord.network/#/explorer</t>
+  </si>
+  <si>
+    <t>https://github.com/dhiway/cord/tree/ondc-hackathon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes </t>
+  </si>
+  <si>
+    <t>https://github.com/dhiway/innovation-hackathon-jan22/blob/main/dhiway/CORD_Lightpaper_v1.pdf</t>
+  </si>
+  <si>
     <t>Beckn Protocol Evolution</t>
   </si>
   <si>
@@ -154,7 +169,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -205,7 +220,14 @@
     </font>
     <font>
       <u/>
+      <sz val="9.0"/>
       <color rgb="FF1155CC"/>
+      <name val="Lato"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9.0"/>
+      <color rgb="FF0000FF"/>
       <name val="Lato"/>
     </font>
     <font>
@@ -516,12 +538,12 @@
     <xf borderId="4" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="4" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1146,21 +1168,21 @@
         <v>26</v>
       </c>
       <c r="I9" s="36" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J9" s="37" t="s">
         <v>24</v>
       </c>
       <c r="K9" s="37" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L9" s="37" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="M9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="N9" s="37" t="s">
+      <c r="N9" s="38" t="s">
         <v>29</v>
       </c>
       <c r="O9" s="22"/>
@@ -1184,9 +1206,9 @@
       <c r="AG9" s="22"/>
     </row>
     <row r="10">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
       <c r="D10" s="31" t="s">
         <v>30</v>
       </c>
@@ -1196,14 +1218,14 @@
       <c r="F10" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
       <c r="O10" s="22"/>
       <c r="P10" s="22"/>
       <c r="Q10" s="22"/>
@@ -1225,9 +1247,9 @@
       <c r="AG10" s="22"/>
     </row>
     <row r="11">
-      <c r="A11" s="38"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
       <c r="D11" s="31" t="s">
         <v>31</v>
       </c>
@@ -1237,14 +1259,14 @@
       <c r="F11" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
       <c r="O11" s="22"/>
       <c r="P11" s="22"/>
       <c r="Q11" s="22"/>
@@ -1266,24 +1288,26 @@
       <c r="AG11" s="22"/>
     </row>
     <row r="12">
-      <c r="A12" s="39"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
       <c r="D12" s="31" t="s">
         <v>32</v>
       </c>
       <c r="E12" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="40"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
+      <c r="F12" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="40"/>
       <c r="O12" s="22"/>
       <c r="P12" s="22"/>
       <c r="Q12" s="22"/>
@@ -1355,15 +1379,33 @@
       <c r="E14" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="40"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="42"/>
-      <c r="N14" s="42"/>
+      <c r="F14" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="L14" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="M14" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="N14" s="36" t="s">
+        <v>40</v>
+      </c>
       <c r="O14" s="22"/>
       <c r="P14" s="22"/>
       <c r="Q14" s="22"/>
@@ -1385,24 +1427,26 @@
       <c r="AG14" s="22"/>
     </row>
     <row r="15">
-      <c r="A15" s="38"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
       <c r="D15" s="31" t="s">
         <v>30</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="40"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="38"/>
+      <c r="F15" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="39"/>
+      <c r="N15" s="39"/>
       <c r="O15" s="22"/>
       <c r="P15" s="22"/>
       <c r="Q15" s="22"/>
@@ -1424,24 +1468,26 @@
       <c r="AG15" s="22"/>
     </row>
     <row r="16">
-      <c r="A16" s="38"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
+      <c r="A16" s="39"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
       <c r="D16" s="31" t="s">
         <v>31</v>
       </c>
       <c r="E16" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="40"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="38"/>
-      <c r="M16" s="38"/>
-      <c r="N16" s="38"/>
+      <c r="F16" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
       <c r="O16" s="22"/>
       <c r="P16" s="22"/>
       <c r="Q16" s="22"/>
@@ -1463,24 +1509,26 @@
       <c r="AG16" s="22"/>
     </row>
     <row r="17">
-      <c r="A17" s="39"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
       <c r="D17" s="31" t="s">
         <v>32</v>
       </c>
       <c r="E17" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="40"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="39"/>
+      <c r="F17" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="40"/>
       <c r="O17" s="22"/>
       <c r="P17" s="22"/>
       <c r="Q17" s="22"/>
@@ -1541,10 +1589,10 @@
         <v>11.0</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D19" s="31" t="s">
         <v>22</v>
@@ -1582,9 +1630,9 @@
       <c r="AG19" s="22"/>
     </row>
     <row r="20">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
       <c r="D20" s="31" t="s">
         <v>30</v>
       </c>
@@ -1592,14 +1640,14 @@
         <v>23</v>
       </c>
       <c r="F20" s="35"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="38"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="39"/>
       <c r="O20" s="22"/>
       <c r="P20" s="22"/>
       <c r="Q20" s="22"/>
@@ -1621,9 +1669,9 @@
       <c r="AG20" s="22"/>
     </row>
     <row r="21">
-      <c r="A21" s="38"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
+      <c r="A21" s="39"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
       <c r="D21" s="31" t="s">
         <v>31</v>
       </c>
@@ -1631,14 +1679,14 @@
         <v>23</v>
       </c>
       <c r="F21" s="35"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="38"/>
-      <c r="L21" s="38"/>
-      <c r="M21" s="38"/>
-      <c r="N21" s="38"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
       <c r="O21" s="22"/>
       <c r="P21" s="22"/>
       <c r="Q21" s="22"/>
@@ -1660,9 +1708,9 @@
       <c r="AG21" s="22"/>
     </row>
     <row r="22">
-      <c r="A22" s="38"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="38"/>
+      <c r="A22" s="39"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
       <c r="D22" s="31" t="s">
         <v>32</v>
       </c>
@@ -1670,14 +1718,14 @@
         <v>23</v>
       </c>
       <c r="F22" s="35"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="38"/>
-      <c r="M22" s="38"/>
-      <c r="N22" s="38"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="39"/>
       <c r="O22" s="22"/>
       <c r="P22" s="22"/>
       <c r="Q22" s="22"/>
@@ -1699,24 +1747,24 @@
       <c r="AG22" s="22"/>
     </row>
     <row r="23">
-      <c r="A23" s="38"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
+      <c r="A23" s="39"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
       <c r="D23" s="31" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E23" s="31" t="s">
         <v>23</v>
       </c>
       <c r="F23" s="35"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="38"/>
-      <c r="K23" s="38"/>
-      <c r="L23" s="38"/>
-      <c r="M23" s="38"/>
-      <c r="N23" s="38"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="39"/>
       <c r="O23" s="22"/>
       <c r="P23" s="22"/>
       <c r="Q23" s="22"/>
@@ -1738,24 +1786,24 @@
       <c r="AG23" s="22"/>
     </row>
     <row r="24">
-      <c r="A24" s="39"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
       <c r="D24" s="31" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E24" s="31" t="s">
         <v>23</v>
       </c>
       <c r="F24" s="35"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="39"/>
-      <c r="N24" s="39"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="40"/>
       <c r="O24" s="22"/>
       <c r="P24" s="22"/>
       <c r="Q24" s="22"/>
@@ -35758,7 +35806,12 @@
     <hyperlink r:id="rId2" ref="G9"/>
     <hyperlink r:id="rId3" ref="H9"/>
     <hyperlink r:id="rId4" ref="I9"/>
+    <hyperlink r:id="rId5" location="network-operations" ref="N9"/>
+    <hyperlink r:id="rId6" location="assumptions" ref="G14"/>
+    <hyperlink r:id="rId7" location="/explorer" ref="H14"/>
+    <hyperlink r:id="rId8" ref="I14"/>
+    <hyperlink r:id="rId9" ref="N14"/>
   </hyperlinks>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>